<commit_message>
[minor] Cleanup and fixed broken redirect.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\Personal\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CECAC39-66B2-4C95-B91B-E30440FDB08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF2E20E-0A34-427A-AABB-21D741323115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Model Used</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Time Series Forecasting</t>
+  </si>
+  <si>
+    <t>Gaussian Naïve Bayes</t>
+  </si>
+  <si>
+    <t>Bank Client Term Deposit</t>
   </si>
 </sst>
 </file>
@@ -289,6 +295,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -296,15 +311,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -621,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -639,7 +645,7 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -650,7 +656,7 @@
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -661,7 +667,7 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -672,7 +678,7 @@
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -683,7 +689,7 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -691,84 +697,96 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="13" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{35050E6F-7EB8-41D3-85AC-70FDEBB1BFBC}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C4" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
+    <hyperlink ref="C6" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Unsupervised Clustering - DBScan - National Health and Nutrition Examination Survey (NHANES).
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\Personal\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF2E20E-0A34-427A-AABB-21D741323115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BCC83D-7243-4E7E-A2EC-212B552D28E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Model Used</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Bank Client Term Deposit</t>
+  </si>
+  <si>
+    <t>Unsupervised Clustering</t>
+  </si>
+  <si>
+    <t>Density-Based Spatial Clustering of Applications with Noise (DBSCAN)</t>
+  </si>
+  <si>
+    <t>National Health and Nutrition Examination Survey (NHANES)</t>
   </si>
 </sst>
 </file>
@@ -265,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,6 +312,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -311,6 +323,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -627,17 +642,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43" style="5"/>
+    <col min="1" max="1" width="50.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="43" style="1"/>
   </cols>
   <sheetData>
@@ -708,7 +723,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -719,7 +734,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
@@ -728,7 +743,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -739,7 +754,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
@@ -747,23 +762,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
       <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -771,7 +797,7 @@
   <mergeCells count="3">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -781,12 +807,13 @@
     <hyperlink ref="C8" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C10" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C12" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C4" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C6" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
+    <hyperlink ref="C11" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Time Series Forecasting - Oil Prices.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\Personal\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BCC83D-7243-4E7E-A2EC-212B552D28E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF552945-1A96-46E9-8500-77F92BBDE8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Model Used</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>National Health and Nutrition Examination Survey (NHANES)</t>
+  </si>
+  <si>
+    <t>Stacked Ensemble (Random Forest Regressor Meta-Learner on SARIMAX and Holt-Winters Models).</t>
+  </si>
+  <si>
+    <t>Oil Prices</t>
   </si>
 </sst>
 </file>
@@ -274,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -315,6 +321,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -324,8 +333,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -642,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -723,7 +732,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -734,7 +743,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
@@ -743,7 +752,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -754,7 +763,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
@@ -769,12 +778,12 @@
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -785,12 +794,23 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -812,8 +832,9 @@
     <hyperlink ref="C4" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C6" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
     <hyperlink ref="C11" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] SARIMAX - Mindtree Stock Price.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\Personal\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF809DE-A6B9-45A3-957A-4DAA8BD0DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1C8CD7-456D-432A-8A06-2C3B7677986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Model Used</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Laptop Price Analysis</t>
+  </si>
+  <si>
+    <t>Seasonal AutoRegressive Integrated Moving Average with eXogenous factors (SARIMAX)</t>
+  </si>
+  <si>
+    <t>Mindtree Stock Price</t>
   </si>
 </sst>
 </file>
@@ -310,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -368,6 +374,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -684,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -854,13 +863,24 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>27</v>
+      <c r="A16" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -884,10 +904,11 @@
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C8" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
     <hyperlink ref="C13" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C16" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C17" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Regression & Binary Classification - Possum Morphometric Analysis.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\Personal\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1C8CD7-456D-432A-8A06-2C3B7677986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC989BC-43D2-4DB7-8503-8B2347F78DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Model Used</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Mindtree Stock Price</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>Possum Morphometric Analysis</t>
   </si>
 </sst>
 </file>
@@ -363,6 +369,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -374,9 +383,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -708,11 +714,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -770,145 +776,169 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
+      <c r="A7" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
+      <c r="A8" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>6</v>
+      <c r="A9" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>7</v>
+      <c r="A11" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>33</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>27</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
       <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{35050E6F-7EB8-41D3-85AC-70FDEBB1BFBC}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
-    <hyperlink ref="C11" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C14" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C15" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
-    <hyperlink ref="C8" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C13" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C17" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C10" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
+    <hyperlink ref="C15" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
+    <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Unsupervised Learning - Relay States - Agglomerative Clustering.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB694C80-2E92-40EB-BBB6-6174304BA57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F902D21-70C7-4313-BC3A-C191BB05D14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Model Used</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Relay States</t>
+  </si>
+  <si>
+    <t>Agglomerative (Hierarchical) Clustering</t>
   </si>
 </sst>
 </file>
@@ -416,6 +419,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,12 +443,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -757,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -772,11 +775,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -878,7 +881,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -889,7 +892,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
@@ -898,7 +901,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -909,7 +912,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
@@ -918,7 +921,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
@@ -927,7 +930,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+      <c r="A16" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
@@ -936,62 +941,73 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
       <c r="B19" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>32</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>26</v>
+      <c r="A21" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A13:A15"/>
   </mergeCells>
@@ -1003,19 +1019,21 @@
     <hyperlink ref="C12" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C15" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C18" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C19" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C10" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C17" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C21" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C18" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C13" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
+    <hyperlink ref="C16" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C17" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Binary Classification - Industrial System Monitoring - Support Vector Classifier.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F902D21-70C7-4313-BC3A-C191BB05D14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A885F-93E8-4CF5-8785-A97BDB8B1962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Model Used</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Agglomerative (Hierarchical) Clustering</t>
+  </si>
+  <si>
+    <t>Industrial System Monitoring</t>
+  </si>
+  <si>
+    <t>Support Vector Classifier (SVC)</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -930,84 +936,95 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>24</v>
+      <c r="A18" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>32</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
       <c r="B21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>26</v>
+      <c r="A22" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A13:A15"/>
   </mergeCells>
@@ -1019,21 +1036,22 @@
     <hyperlink ref="C12" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C15" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C19" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C20" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C21" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C10" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C18" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C22" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C19" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C23" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C21" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C22" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C13" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C16" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C17" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C17" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C18" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C16" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Classification - Brain Stroke Prediction - Voting Classifier.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A885F-93E8-4CF5-8785-A97BDB8B1962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BEF189-3554-42B6-A164-3B2F2DD97902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Model Used</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Support Vector Classifier (SVC)</t>
+  </si>
+  <si>
+    <t>Brain Stroke</t>
+  </si>
+  <si>
+    <t>Voting Classifier - (XGBoost, Random Forest) with Logistic Regression as meta-model.</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -450,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -935,96 +944,107 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>42</v>
+    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>44</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
-        <v>24</v>
+      <c r="A19" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
       <c r="B21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>32</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>26</v>
+      <c r="A23" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A13:A15"/>
   </mergeCells>
@@ -1036,22 +1056,23 @@
     <hyperlink ref="C12" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C15" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C20" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C21" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C21" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C22" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C10" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C19" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C23" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C20" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C24" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C22" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C23" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C13" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C17" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C18" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
-    <hyperlink ref="C16" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
+    <hyperlink ref="C18" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C17" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
+    <hyperlink ref="C16" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Classification - Loan Prediction - Logistic Regression.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BEF189-3554-42B6-A164-3B2F2DD97902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC359B-A781-46A4-9C7F-E35981613F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Model Used</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Voting Classifier - (XGBoost, Random Forest) with Logistic Regression as meta-model.</t>
+  </si>
+  <si>
+    <t>Loan Prediction</t>
   </si>
 </sst>
 </file>
@@ -436,6 +439,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -456,9 +462,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -775,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -790,11 +793,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -874,7 +877,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -885,54 +888,54 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A10" s="26"/>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>6</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20" t="s">
+        <v>6</v>
+      </c>
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="20"/>
       <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -941,138 +944,149 @@
         <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
-        <v>44</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
       <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>24</v>
+      <c r="A20" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>32</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>26</v>
+      <c r="A24" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A21:A22"/>
+  <mergeCells count="5">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{35050E6F-7EB8-41D3-85AC-70FDEBB1BFBC}"/>
     <hyperlink ref="C9" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
-    <hyperlink ref="C12" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
-    <hyperlink ref="C15" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C21" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C22" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
+    <hyperlink ref="C22" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C23" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C20" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C24" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
+    <hyperlink ref="C21" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C25" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C23" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C24" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
-    <hyperlink ref="C13" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C18" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C19" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
-    <hyperlink ref="C17" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
-    <hyperlink ref="C16" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
+    <hyperlink ref="C14" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C18" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
+    <hyperlink ref="C17" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
+    <hyperlink ref="C10" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Classification - Churn Prediction - Random Forest Classifier.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC359B-A781-46A4-9C7F-E35981613F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8781B-F634-4F1E-9B10-78EE95D87C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Model Used</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>Loan Prediction</t>
+  </si>
+  <si>
+    <t>Churn Prediction</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -375,6 +378,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -383,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -412,15 +428,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -433,9 +443,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -462,6 +469,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -778,32 +806,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="43" style="1"/>
+    <col min="1" max="1" width="42.109375" style="5"/>
+    <col min="2" max="2" width="42.109375" style="4"/>
+    <col min="3" max="16384" width="42.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -814,7 +841,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -825,9 +852,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="27"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -836,18 +861,16 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="B5" s="26"/>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -855,21 +878,17 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="A7" s="23"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -877,216 +896,203 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="14" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="19"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
+    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
+  <mergeCells count="12">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{35050E6F-7EB8-41D3-85AC-70FDEBB1BFBC}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
-    <hyperlink ref="C15" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
-    <hyperlink ref="C16" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C22" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C23" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
+    <hyperlink ref="C13" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
+    <hyperlink ref="C16" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
+    <hyperlink ref="C17" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
+    <hyperlink ref="C23" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C24" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C21" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C25" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
+    <hyperlink ref="C22" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C26" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C24" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C25" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
-    <hyperlink ref="C14" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C19" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C20" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
-    <hyperlink ref="C18" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
-    <hyperlink ref="C17" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
-    <hyperlink ref="C10" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
+    <hyperlink ref="C15" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C19" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
+    <hyperlink ref="C18" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
+    <hyperlink ref="C11" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
+    <hyperlink ref="C9" r:id="rId24" xr:uid="{F8FC8A11-DB79-492E-9C67-E9AC9A4D5434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Classification - Chronic Kidney Disease Classification - Gaussian Naive Bayes.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8781B-F634-4F1E-9B10-78EE95D87C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7C077-279A-4C2F-8AB3-8F6997A28E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Model Used</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Churn Prediction</t>
+  </si>
+  <si>
+    <t>Stroke Prediction</t>
+  </si>
+  <si>
+    <t>Chronic Kidney Disease Classification</t>
   </si>
 </sst>
 </file>
@@ -450,6 +456,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -470,16 +479,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -806,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -820,11 +826,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -852,7 +858,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -861,13 +867,13 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="25" t="s">
@@ -878,14 +884,14 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -897,202 +903,219 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="2" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="2" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="2" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="2" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="2" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A19" s="24"/>
       <c r="B19" s="26"/>
       <c r="C19" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>38</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="26"/>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B23" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="12" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>26</v>
-      </c>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
       <c r="B26" s="26"/>
       <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A23:A24"/>
+  <mergeCells count="13">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B8:B21"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{35050E6F-7EB8-41D3-85AC-70FDEBB1BFBC}"/>
-    <hyperlink ref="C10" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
-    <hyperlink ref="C13" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
-    <hyperlink ref="C14" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
-    <hyperlink ref="C16" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
-    <hyperlink ref="C17" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C23" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C24" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{761B161E-57FB-4875-9D72-DB299E0CB342}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{406C3342-512C-43EA-9A8F-21A724D909B1}"/>
+    <hyperlink ref="C16" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
+    <hyperlink ref="C25" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C26" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C22" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C26" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
+    <hyperlink ref="C24" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C28" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C25" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C27" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
-    <hyperlink ref="C15" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
-    <hyperlink ref="C19" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
-    <hyperlink ref="C18" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
-    <hyperlink ref="C11" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C23" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
+    <hyperlink ref="C20" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
+    <hyperlink ref="C12" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
     <hyperlink ref="C9" r:id="rId24" xr:uid="{F8FC8A11-DB79-492E-9C67-E9AC9A4D5434}"/>
+    <hyperlink ref="C10" r:id="rId25" xr:uid="{C9D46457-1644-42E9-8710-15ADCA4B7BB4}"/>
+    <hyperlink ref="C14" r:id="rId26" xr:uid="{9375C94A-B7F6-40B6-85A8-914D0BD38D8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Clustering - Credit Card Clustering - K-Means Algorithm.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7C077-279A-4C2F-8AB3-8F6997A28E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0CFADA-9032-4016-A61F-EA4B649AA060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Model Used</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Chronic Kidney Disease Classification</t>
+  </si>
+  <si>
+    <t>K-Means Clustering</t>
+  </si>
+  <si>
+    <t>Credit Card Clustering</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -496,6 +502,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -812,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1017,75 +1026,84 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="12" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B26" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>32</v>
-      </c>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
       <c r="B27" s="26"/>
       <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+    <row r="29" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="2" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B8:B21"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B26:B29"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B23:B25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -1095,27 +1113,28 @@
     <hyperlink ref="C16" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C18" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C19" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C25" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C26" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C26" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C27" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C24" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C28" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C25" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C29" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C27" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C28" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
     <hyperlink ref="C22" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C23" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C24" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
     <hyperlink ref="C21" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
     <hyperlink ref="C20" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
     <hyperlink ref="C12" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
     <hyperlink ref="C9" r:id="rId24" xr:uid="{F8FC8A11-DB79-492E-9C67-E9AC9A4D5434}"/>
     <hyperlink ref="C10" r:id="rId25" xr:uid="{C9D46457-1644-42E9-8710-15ADCA4B7BB4}"/>
     <hyperlink ref="C14" r:id="rId26" xr:uid="{9375C94A-B7F6-40B6-85A8-914D0BD38D8D}"/>
+    <hyperlink ref="C23" r:id="rId27" xr:uid="{51F8C9B9-B18E-40E9-8546-2DF0F93C7F5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Clustering - Breast Cancer - Agglomerative Clustering.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0CFADA-9032-4016-A61F-EA4B649AA060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCBE477-F24E-471A-A17D-1283762525C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Model Used</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Credit Card Clustering</t>
+  </si>
+  <si>
+    <t>Breast Cancer Clustering</t>
   </si>
 </sst>
 </file>
@@ -494,16 +497,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -821,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -856,7 +859,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1028,82 +1031,90 @@
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="31"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="12" t="s">
+      <c r="B26" s="31"/>
+      <c r="C26" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B27" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>32</v>
-      </c>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
       <c r="B28" s="26"/>
       <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+    <row r="30" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="2" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A27:A28"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B8:B21"/>
-    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B27:B30"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -1113,19 +1124,19 @@
     <hyperlink ref="C16" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C18" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C19" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C26" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C27" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C27" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C28" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C25" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C29" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C26" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C30" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C28" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C29" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
     <hyperlink ref="C22" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C24" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C25" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
     <hyperlink ref="C21" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
     <hyperlink ref="C20" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
     <hyperlink ref="C12" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
@@ -1133,8 +1144,9 @@
     <hyperlink ref="C10" r:id="rId25" xr:uid="{C9D46457-1644-42E9-8710-15ADCA4B7BB4}"/>
     <hyperlink ref="C14" r:id="rId26" xr:uid="{9375C94A-B7F6-40B6-85A8-914D0BD38D8D}"/>
     <hyperlink ref="C23" r:id="rId27" xr:uid="{51F8C9B9-B18E-40E9-8546-2DF0F93C7F5F}"/>
+    <hyperlink ref="C24" r:id="rId28" xr:uid="{A296EDA1-4AC0-4AAD-A3A5-5982E4B6E49C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Clustering - Penguin Morphological Analysis - KMeans, Agglomerative & DBScan Clustering.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCBE477-F24E-471A-A17D-1283762525C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A997E0C9-0467-48DF-AF0A-DBD7093154C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Model Used</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Breast Cancer Clustering</t>
+  </si>
+  <si>
+    <t>Penguin Morphological Analysis</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -446,68 +449,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -824,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -838,11 +847,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -859,7 +868,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -870,7 +879,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -879,16 +888,16 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -896,17 +905,17 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -914,95 +923,95 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
@@ -1011,27 +1020,27 @@
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1039,82 +1048,105 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="2" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="2" t="s">
+    <row r="26" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="31"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="12" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="33"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="2" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="2" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+    <row r="33" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="2" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B8:B21"/>
-    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -1124,19 +1156,19 @@
     <hyperlink ref="C16" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C18" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C19" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C27" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C28" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C30" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C31" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C26" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C30" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C28" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C33" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C29" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C32" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
     <hyperlink ref="C22" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C25" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C26" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
     <hyperlink ref="C21" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
     <hyperlink ref="C20" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
     <hyperlink ref="C12" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
@@ -1144,9 +1176,12 @@
     <hyperlink ref="C10" r:id="rId25" xr:uid="{C9D46457-1644-42E9-8710-15ADCA4B7BB4}"/>
     <hyperlink ref="C14" r:id="rId26" xr:uid="{9375C94A-B7F6-40B6-85A8-914D0BD38D8D}"/>
     <hyperlink ref="C23" r:id="rId27" xr:uid="{51F8C9B9-B18E-40E9-8546-2DF0F93C7F5F}"/>
-    <hyperlink ref="C24" r:id="rId28" xr:uid="{A296EDA1-4AC0-4AAD-A3A5-5982E4B6E49C}"/>
+    <hyperlink ref="C25" r:id="rId28" xr:uid="{A296EDA1-4AC0-4AAD-A3A5-5982E4B6E49C}"/>
+    <hyperlink ref="C24" r:id="rId29" xr:uid="{301C0257-4326-4070-B474-22A9875ED3AD}"/>
+    <hyperlink ref="C27" r:id="rId30" xr:uid="{9FBEECA7-BACE-41E6-829A-60DA30E76ADF}"/>
+    <hyperlink ref="C29" r:id="rId31" xr:uid="{1E9A6F4D-F860-4C0D-98E9-7F24F0960D44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Classification & Clustering - Human Activity Recognition.ipynb - Random Forest Classifier & Agglomerative Clustering.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A997E0C9-0467-48DF-AF0A-DBD7093154C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A7D757-2D08-4208-B493-15D94395AD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Model Used</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Penguin Morphological Analysis</t>
+  </si>
+  <si>
+    <t>Human Activity Recognition</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -458,65 +461,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C29" activeCellId="1" sqref="C22 C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -847,11 +844,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -868,7 +865,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -879,7 +876,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -888,16 +885,16 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -905,17 +902,17 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -923,95 +920,95 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="25"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
@@ -1020,133 +1017,149 @@
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+    <row r="24" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B24" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="2" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="2" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="2" t="s">
+    <row r="27" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="2" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="31"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="22"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="11" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="33"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="22"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="2" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+    <row r="35" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="2" t="s">
+      <c r="B35" s="29"/>
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="A28:A29"/>
+  <mergeCells count="18">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B24:B31"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B8:B21"/>
-    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B32:B35"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -1156,32 +1169,34 @@
     <hyperlink ref="C16" r:id="rId5" xr:uid="{3B4DAEE7-C0AF-4F31-AA8C-2C266F09EE48}"/>
     <hyperlink ref="C18" r:id="rId6" xr:uid="{8434BC92-FD37-420A-A9A5-74028AE21620}"/>
     <hyperlink ref="C19" r:id="rId7" xr:uid="{B96CD50F-6B31-45BC-83BA-5D0C8CBB95C7}"/>
-    <hyperlink ref="C30" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
-    <hyperlink ref="C31" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
+    <hyperlink ref="C32" r:id="rId8" xr:uid="{94F7CDF6-1AC6-4474-8328-8204642BD74B}"/>
+    <hyperlink ref="C33" r:id="rId9" xr:uid="{C7BEE59B-970F-403D-BCD9-04C404B07AE9}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
-    <hyperlink ref="C28" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C33" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C30" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
+    <hyperlink ref="C35" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C32" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C34" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
-    <hyperlink ref="C22" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
-    <hyperlink ref="C26" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
+    <hyperlink ref="C23" r:id="rId19" xr:uid="{F94B4234-757B-4513-9321-3D711E52AC95}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{582D36C4-0CCC-48D3-BA48-4011DA044A88}"/>
     <hyperlink ref="C21" r:id="rId21" xr:uid="{1F17CCE3-4526-44B7-8B19-EA501209CB2E}"/>
     <hyperlink ref="C20" r:id="rId22" xr:uid="{26906615-F509-473B-8D35-EF617A67E689}"/>
     <hyperlink ref="C12" r:id="rId23" xr:uid="{25AEB3C5-5389-434C-9122-E3C13FB5CE5C}"/>
     <hyperlink ref="C9" r:id="rId24" xr:uid="{F8FC8A11-DB79-492E-9C67-E9AC9A4D5434}"/>
     <hyperlink ref="C10" r:id="rId25" xr:uid="{C9D46457-1644-42E9-8710-15ADCA4B7BB4}"/>
     <hyperlink ref="C14" r:id="rId26" xr:uid="{9375C94A-B7F6-40B6-85A8-914D0BD38D8D}"/>
-    <hyperlink ref="C23" r:id="rId27" xr:uid="{51F8C9B9-B18E-40E9-8546-2DF0F93C7F5F}"/>
-    <hyperlink ref="C25" r:id="rId28" xr:uid="{A296EDA1-4AC0-4AAD-A3A5-5982E4B6E49C}"/>
-    <hyperlink ref="C24" r:id="rId29" xr:uid="{301C0257-4326-4070-B474-22A9875ED3AD}"/>
-    <hyperlink ref="C27" r:id="rId30" xr:uid="{9FBEECA7-BACE-41E6-829A-60DA30E76ADF}"/>
-    <hyperlink ref="C29" r:id="rId31" xr:uid="{1E9A6F4D-F860-4C0D-98E9-7F24F0960D44}"/>
+    <hyperlink ref="C24" r:id="rId27" xr:uid="{51F8C9B9-B18E-40E9-8546-2DF0F93C7F5F}"/>
+    <hyperlink ref="C26" r:id="rId28" xr:uid="{A296EDA1-4AC0-4AAD-A3A5-5982E4B6E49C}"/>
+    <hyperlink ref="C25" r:id="rId29" xr:uid="{301C0257-4326-4070-B474-22A9875ED3AD}"/>
+    <hyperlink ref="C28" r:id="rId30" xr:uid="{9FBEECA7-BACE-41E6-829A-60DA30E76ADF}"/>
+    <hyperlink ref="C31" r:id="rId31" xr:uid="{1E9A6F4D-F860-4C0D-98E9-7F24F0960D44}"/>
+    <hyperlink ref="C29" r:id="rId32" xr:uid="{D0612C45-499E-409E-8B7C-17D21F1D86CE}"/>
+    <hyperlink ref="C22" r:id="rId33" xr:uid="{EBA3F891-6FA1-43A0-BA87-7F332F1E9F96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[minor] Time Series Forecasting - Electricity Demand - SARIMAX.
</commit_message>
<xml_diff>
--- a/Models Used.xlsx
+++ b/Models Used.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aditya Sreevatsa K\Repositories\DS_ML_Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A7D757-2D08-4208-B493-15D94395AD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20D7BC3-B170-4BF1-9DF2-D98EA95F7949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A27EBF2-D7E0-4B73-8606-34D19F158E24}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Model Used</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>Human Activity Recognition</t>
+  </si>
+  <si>
+    <t>Shampoo Sales</t>
+  </si>
+  <si>
+    <t>Retail Sales</t>
+  </si>
+  <si>
+    <t>Electricity Demand</t>
   </si>
 </sst>
 </file>
@@ -455,39 +464,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,20 +512,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -830,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B504DA7A-9582-47E2-8A3A-5A53DC2E9F07}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C29" activeCellId="1" sqref="C22 C29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -844,11 +853,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -865,7 +874,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -885,16 +894,16 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -902,17 +911,17 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -920,21 +929,21 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="28"/>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="28"/>
       <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="28"/>
@@ -943,14 +952,14 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="28"/>
       <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="28"/>
@@ -959,14 +968,14 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="28"/>
       <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="28"/>
@@ -975,14 +984,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="28"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="28"/>
@@ -991,21 +1000,21 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="28"/>
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="28"/>
@@ -1017,16 +1026,16 @@
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1034,17 +1043,17 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1052,63 +1061,63 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1116,50 +1125,72 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="2" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="2" t="s">
+      <c r="B38" s="31"/>
+      <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B24:B31"/>
-    <mergeCell ref="A30:A31"/>
+  <mergeCells count="19">
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A32:A33"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B8:B21"/>
-    <mergeCell ref="B32:B35"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B24:B31"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{305F0E37-899F-4FD0-9229-EC28109BEAC6}"/>
@@ -1174,9 +1205,9 @@
     <hyperlink ref="C5" r:id="rId10" xr:uid="{925176A7-B0C3-40DE-BE1B-53BCF9CF6851}"/>
     <hyperlink ref="C13" r:id="rId11" xr:uid="{73B62350-A3B2-40EC-88E6-35D0CC21B6C4}"/>
     <hyperlink ref="C30" r:id="rId12" display="NHANES" xr:uid="{B2F76FAE-E40F-40A0-81CB-7D2072C18F71}"/>
-    <hyperlink ref="C35" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
+    <hyperlink ref="C38" r:id="rId13" xr:uid="{0D8B383D-B1EA-4C78-874D-C1D57BDE0281}"/>
     <hyperlink ref="C6" r:id="rId14" xr:uid="{46D19442-1FD8-4D8C-9486-92A79DF810FD}"/>
-    <hyperlink ref="C34" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
+    <hyperlink ref="C36" r:id="rId15" xr:uid="{4A5D421C-5068-46C8-8560-18E9BFEE5DA3}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{587AC6CB-29B4-488D-99CA-C3AF7C2847E6}"/>
     <hyperlink ref="C8" r:id="rId17" xr:uid="{7A8D1835-E9DC-4E8E-B3CB-21FA8A932D8A}"/>
     <hyperlink ref="C17" r:id="rId18" xr:uid="{1CA34B06-5E6C-4435-AF30-6AA8C4DEEC13}"/>
@@ -1195,8 +1226,11 @@
     <hyperlink ref="C31" r:id="rId31" xr:uid="{1E9A6F4D-F860-4C0D-98E9-7F24F0960D44}"/>
     <hyperlink ref="C29" r:id="rId32" xr:uid="{D0612C45-499E-409E-8B7C-17D21F1D86CE}"/>
     <hyperlink ref="C22" r:id="rId33" xr:uid="{EBA3F891-6FA1-43A0-BA87-7F332F1E9F96}"/>
+    <hyperlink ref="C34" r:id="rId34" xr:uid="{F7CBCE06-642D-4B61-8BE4-928AD3B33CEB}"/>
+    <hyperlink ref="C35" r:id="rId35" xr:uid="{0A3152C3-45A4-4579-A311-870A7696F142}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{4EF0D791-E771-42DF-9350-C88887F6A2BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>